<commit_message>
test data sequence is changed
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-RequestForInformation-CancelAndClose.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-RequestForInformation-CancelAndClose.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -502,7 +502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -599,7 +601,7 @@
         <v>5</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -628,7 +630,7 @@
         <v>5</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:16">

</xml_diff>